<commit_message>
Added thumbnail loading gallery
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48815bcfcfd05c63/Coding/Python/repository/cornandcheese/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsnar\OneDrive\Coding\Python\repository\cornandcheese\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{BAEA6321-44CF-4447-BEDE-114931F5D5A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9878" xr2:uid="{0D853D45-DFB9-4809-8CD0-306EA965E176}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9878" xr2:uid="{0D853D45-DFB9-4809-8CD0-306EA965E176}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>